<commit_message>
Correcciones de 3-4 ciclo de para calidad
</commit_message>
<xml_diff>
--- a/docs/Funcionalidades evac.xlsx
+++ b/docs/Funcionalidades evac.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6375" windowWidth="28830" windowHeight="3195"/>
+    <workbookView xWindow="-15" yWindow="6435" windowWidth="28830" windowHeight="3135"/>
   </bookViews>
   <sheets>
     <sheet name="Fechas de Entregas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="104">
   <si>
     <t>OPERATIVO</t>
   </si>
@@ -293,6 +293,45 @@
   </si>
   <si>
     <t>Auditoria caratula listo</t>
+  </si>
+  <si>
+    <t>FU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO99 = </t>
+  </si>
+  <si>
+    <t>Formulario borrador</t>
+  </si>
+  <si>
+    <t>Manual de diligenciamiento</t>
+  </si>
+  <si>
+    <t>Glosario de terminsos</t>
+  </si>
+  <si>
+    <t>DIRECTORIO DE EMPRESAS</t>
+  </si>
+  <si>
+    <t>CAPITULO I</t>
+  </si>
+  <si>
+    <t>OBSERVACIONES CRÍTICO</t>
+  </si>
+  <si>
+    <t>LISTADO DE ACTIVIDADES</t>
+  </si>
+  <si>
+    <t>TABLA DE CONTROL</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>ext</t>
+  </si>
+  <si>
+    <t>Manual Critica</t>
   </si>
 </sst>
 </file>
@@ -425,7 +464,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -638,6 +677,59 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -648,7 +740,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -731,51 +823,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -783,9 +875,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -803,13 +892,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1119,40 +1230,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="B10:C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="119.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="62">
         <v>42587</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="63">
         <v>42587</v>
       </c>
       <c r="E4" t="s">
@@ -1161,37 +1274,37 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="63">
         <v>42587</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="64">
         <v>42587</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="65">
         <v>42594</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="63">
         <v>42594</v>
       </c>
       <c r="E8" t="s">
@@ -1203,119 +1316,170 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="63">
         <v>42594</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="64">
         <v>42594</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="57">
         <v>42601</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="59">
         <v>42601</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="59">
         <v>42601</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="55" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="61">
         <v>42601</v>
+      </c>
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="57">
         <v>42608</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="55" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="59">
         <v>42608</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F16" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="55" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="59">
         <v>42608</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F17" s="55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="61">
         <v>42608</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="29"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="29"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="29"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="29"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="9"/>
     </row>
   </sheetData>
@@ -1344,47 +1508,47 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="43"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="52"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="G3" s="44" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="G3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44" t="s">
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="45"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:16" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="53"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="27" t="s">
         <v>40</v>
       </c>
@@ -1417,7 +1581,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="47" t="s">
@@ -1451,12 +1615,12 @@
       <c r="O5" s="21"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40" t="s">
+      <c r="B6" s="46"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="40"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="6" t="s">
         <v>49</v>
       </c>
@@ -1483,12 +1647,12 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40" t="s">
+      <c r="B7" s="46"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="40"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="6" t="s">
         <v>49</v>
       </c>
@@ -1513,12 +1677,12 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="2:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="49" t="s">
+      <c r="B8" s="46"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="49"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
@@ -1548,14 +1712,14 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="40" t="s">
+      <c r="B9" s="46"/>
+      <c r="C9" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="40"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="6" t="s">
         <v>49</v>
       </c>
@@ -1580,12 +1744,12 @@
       <c r="O9" s="22"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40" t="s">
+      <c r="B10" s="46"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="40"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="6" t="s">
         <v>49</v>
       </c>
@@ -1612,12 +1776,12 @@
       <c r="O10" s="22"/>
     </row>
     <row r="11" spans="2:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="50" t="s">
+      <c r="B11" s="46"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="50"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6" t="s">
@@ -1640,14 +1804,14 @@
       <c r="O11" s="24"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="46" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="6" t="s">
         <v>50</v>
       </c>
@@ -1674,12 +1838,12 @@
       <c r="O12" s="22"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="6" t="s">
         <v>50</v>
       </c>
@@ -1706,14 +1870,14 @@
       <c r="O13" s="22"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
-      <c r="C14" s="40" t="s">
+      <c r="B14" s="46"/>
+      <c r="C14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="57" t="s">
+      <c r="D14" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="57"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="6" t="s">
         <v>50</v>
       </c>
@@ -1744,12 +1908,12 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="49" t="s">
+      <c r="B15" s="46"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="49"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
         <v>50</v>
@@ -1781,12 +1945,12 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1805,12 +1969,12 @@
       <c r="O16" s="22"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
         <v>50</v>
@@ -1835,12 +1999,12 @@
       <c r="O17" s="21"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="41"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
         <v>50</v>
@@ -1865,12 +2029,12 @@
       <c r="O18" s="22"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1889,12 +2053,12 @@
       <c r="O19" s="21"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="41"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6" t="s">
@@ -1917,12 +2081,12 @@
       <c r="O20" s="21"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="41"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -1943,12 +2107,12 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="41"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="6" t="s">
         <v>50</v>
       </c>
@@ -1976,14 +2140,14 @@
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="46" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -2004,12 +2168,12 @@
       <c r="O23" s="21"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="41"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -2030,14 +2194,14 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -2056,12 +2220,12 @@
       <c r="O25" s="24"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="56"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -2080,12 +2244,12 @@
       <c r="O26" s="21"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="56"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -2100,12 +2264,12 @@
       <c r="O27" s="21"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="56"/>
-      <c r="C28" s="35" t="s">
+      <c r="B28" s="36"/>
+      <c r="C28" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -2124,12 +2288,12 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="56"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
       <c r="H29" s="23"/>
@@ -2147,14 +2311,14 @@
       <c r="N29" s="23"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="36" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
       <c r="F30" s="15" t="s">
         <v>50</v>
       </c>
@@ -2184,12 +2348,12 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="56"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
       <c r="F31" s="15" t="s">
         <v>50</v>
       </c>
@@ -2219,12 +2383,12 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="56"/>
+      <c r="B32" s="36"/>
       <c r="C32" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -2238,12 +2402,12 @@
       <c r="N32" s="15"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="56"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
       <c r="F33" s="15" t="s">
         <v>50</v>
       </c>
@@ -2273,12 +2437,12 @@
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="56"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15" t="s">
         <v>49</v>
@@ -2302,12 +2466,12 @@
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="56"/>
+      <c r="B35" s="36"/>
       <c r="C35" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
       <c r="F35" s="15" t="s">
         <v>50</v>
       </c>
@@ -2337,12 +2501,12 @@
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="56"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
       <c r="F36" s="14" t="s">
         <v>50</v>
       </c>
@@ -2361,6 +2525,34 @@
   </sheetData>
   <autoFilter ref="F4:O36"/>
   <mergeCells count="44">
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B12:B22"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F2:N2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B2:E4"/>
     <mergeCell ref="B30:B36"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D14:E14"/>
@@ -2377,34 +2569,6 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F2:N2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B2:E4"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B12:B22"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
@@ -2425,7 +2589,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="34" t="s">
         <v>56</v>
       </c>
       <c r="E2" t="s">
@@ -2433,32 +2597,32 @@
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="35" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="35" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="35" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="35" t="s">
         <v>63</v>
       </c>
       <c r="E8" t="s">
@@ -2466,7 +2630,7 @@
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="35" t="s">
         <v>64</v>
       </c>
       <c r="E9" t="s">
@@ -2474,7 +2638,7 @@
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="35" t="s">
         <v>65</v>
       </c>
       <c r="E10" t="s">
@@ -2482,17 +2646,17 @@
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="35" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="35" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="35" t="s">
         <v>68</v>
       </c>
       <c r="E13" t="s">
@@ -2500,17 +2664,17 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="35" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="35" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="35" t="s">
         <v>71</v>
       </c>
       <c r="E16" t="s">
@@ -2518,7 +2682,7 @@
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="35" t="s">
         <v>72</v>
       </c>
       <c r="E17" t="s">
@@ -2526,22 +2690,22 @@
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="35" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="35" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="35" t="s">
         <v>76</v>
       </c>
       <c r="E21" t="s">
@@ -2549,7 +2713,7 @@
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="35" t="s">
         <v>77</v>
       </c>
       <c r="E22" t="s">
@@ -2557,12 +2721,12 @@
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="35" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="35" t="s">
         <v>79</v>
       </c>
       <c r="E24" t="s">
@@ -2570,12 +2734,12 @@
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="35" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="35" t="s">
         <v>81</v>
       </c>
       <c r="E26" t="s">
@@ -2583,7 +2747,7 @@
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="35" t="s">
         <v>82</v>
       </c>
       <c r="E27" t="s">
@@ -2591,17 +2755,17 @@
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="35" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="35" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="38" t="s">
+      <c r="C30" s="35" t="s">
         <v>85</v>
       </c>
       <c r="E30" t="s">
@@ -2609,7 +2773,7 @@
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="35" t="s">
         <v>86</v>
       </c>
       <c r="E31" t="s">

</xml_diff>

<commit_message>
Documentacion Soporte informatico completa SIN-010-r1, SIN-020-r1, SIN-030-r1, SIN-040-r1,r2,r3
</commit_message>
<xml_diff>
--- a/docs/Funcionalidades evac.xlsx
+++ b/docs/Funcionalidades evac.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="105">
   <si>
     <t>OPERATIVO</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>Manual Critica</t>
+  </si>
+  <si>
+    <t>Este amnual lo hace tematica</t>
   </si>
 </sst>
 </file>
@@ -740,7 +743,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -835,70 +838,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -920,7 +863,76 @@
     <xf numFmtId="14" fontId="10" fillId="3" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1231,7 +1243,7 @@
   <dimension ref="A2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,19 +1265,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="62">
+      <c r="C3" s="42">
         <v>42587</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="63">
+      <c r="C4" s="43">
         <v>42587</v>
       </c>
       <c r="E4" t="s">
@@ -1274,37 +1286,37 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="63">
+      <c r="C5" s="43">
         <v>42587</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="44">
         <v>42587</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="42">
         <v>42594</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="63">
+      <c r="C8" s="43">
         <v>42594</v>
       </c>
       <c r="E8" t="s">
@@ -1316,28 +1328,28 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="63">
+      <c r="C9" s="43">
         <v>42594</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="44">
         <v>42594</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="57">
+      <c r="C11" s="64">
         <v>42601</v>
       </c>
       <c r="E11" t="s">
@@ -1352,106 +1364,109 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="59">
+      <c r="C12" s="65">
         <v>42601</v>
       </c>
       <c r="E12" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="55" t="s">
+      <c r="F12" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="55" t="s">
+      <c r="G12" s="36" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="59">
+      <c r="C13" s="65">
         <v>42601</v>
       </c>
       <c r="E13" t="s">
         <v>94</v>
       </c>
-      <c r="F13" s="55" t="s">
+      <c r="F13" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="G13" s="55" t="s">
+      <c r="G13" s="36" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="61">
+      <c r="C14" s="66">
         <v>42601</v>
       </c>
       <c r="E14" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="G14" s="55" t="s">
+      <c r="G14" s="36" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="57">
+      <c r="C15" s="67">
         <v>42608</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="G15" s="55" t="s">
+      <c r="G15" s="36" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="59">
+      <c r="C16" s="39">
         <v>42608</v>
       </c>
-      <c r="F16" s="55" t="s">
+      <c r="D16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="55" t="s">
+      <c r="G16" s="36" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="59">
+      <c r="C17" s="68">
         <v>42608</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="36" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="61">
+      <c r="C18" s="41">
         <v>42608</v>
       </c>
     </row>
@@ -1508,47 +1523,47 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="48"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="51"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="G3" s="43" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="G3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43" t="s">
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="44"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="50"/>
     </row>
     <row r="4" spans="2:16" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="27" t="s">
         <v>40</v>
       </c>
@@ -1581,16 +1596,16 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="53"/>
       <c r="F5" s="5" t="s">
         <v>49</v>
       </c>
@@ -1616,11 +1631,11 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="46"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37" t="s">
+      <c r="C6" s="45"/>
+      <c r="D6" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="6" t="s">
         <v>49</v>
       </c>
@@ -1648,11 +1663,11 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="46"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37" t="s">
+      <c r="C7" s="45"/>
+      <c r="D7" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="37"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="6" t="s">
         <v>49</v>
       </c>
@@ -1678,11 +1693,11 @@
     </row>
     <row r="8" spans="2:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="46"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="39" t="s">
+      <c r="C8" s="45"/>
+      <c r="D8" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
@@ -1713,13 +1728,13 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="46"/>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="37"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="6" t="s">
         <v>49</v>
       </c>
@@ -1745,11 +1760,11 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="46"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37" t="s">
+      <c r="C10" s="45"/>
+      <c r="D10" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="37"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="6" t="s">
         <v>49</v>
       </c>
@@ -1777,11 +1792,11 @@
     </row>
     <row r="11" spans="2:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="46"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="49" t="s">
+      <c r="C11" s="45"/>
+      <c r="D11" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="49"/>
+      <c r="E11" s="55"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6" t="s">
@@ -1810,8 +1825,8 @@
       <c r="C12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="6" t="s">
         <v>50</v>
       </c>
@@ -1842,8 +1857,8 @@
       <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="6" t="s">
         <v>50</v>
       </c>
@@ -1871,13 +1886,13 @@
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="46"/>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="62"/>
       <c r="F14" s="6" t="s">
         <v>50</v>
       </c>
@@ -1909,11 +1924,11 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="46"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="39" t="s">
+      <c r="C15" s="45"/>
+      <c r="D15" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="54"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
         <v>50</v>
@@ -1949,8 +1964,8 @@
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1973,8 +1988,8 @@
       <c r="C17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
         <v>50</v>
@@ -2003,8 +2018,8 @@
       <c r="C18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
         <v>50</v>
@@ -2033,8 +2048,8 @@
       <c r="C19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -2057,8 +2072,8 @@
       <c r="C20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6" t="s">
@@ -2085,8 +2100,8 @@
       <c r="C21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -2111,8 +2126,8 @@
       <c r="C22" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
       <c r="F22" s="6" t="s">
         <v>50</v>
       </c>
@@ -2146,8 +2161,8 @@
       <c r="C23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -2172,8 +2187,8 @@
       <c r="C24" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -2194,14 +2209,14 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="61" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -2220,12 +2235,12 @@
       <c r="O25" s="24"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="36"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -2244,12 +2259,12 @@
       <c r="O26" s="21"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="36"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -2264,12 +2279,12 @@
       <c r="O27" s="21"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="36"/>
+      <c r="B28" s="61"/>
       <c r="C28" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -2288,12 +2303,12 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="36"/>
+      <c r="B29" s="61"/>
       <c r="C29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
       <c r="H29" s="23"/>
@@ -2311,14 +2326,14 @@
       <c r="N29" s="23"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="61" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
       <c r="F30" s="15" t="s">
         <v>50</v>
       </c>
@@ -2348,12 +2363,12 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="36"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
       <c r="F31" s="15" t="s">
         <v>50</v>
       </c>
@@ -2383,12 +2398,12 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="36"/>
+      <c r="B32" s="61"/>
       <c r="C32" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -2402,12 +2417,12 @@
       <c r="N32" s="15"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="36"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
       <c r="F33" s="15" t="s">
         <v>50</v>
       </c>
@@ -2437,12 +2452,12 @@
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="36"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15" t="s">
         <v>49</v>
@@ -2466,12 +2481,12 @@
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="36"/>
+      <c r="B35" s="61"/>
       <c r="C35" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
       <c r="F35" s="15" t="s">
         <v>50</v>
       </c>
@@ -2501,12 +2516,12 @@
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="36"/>
+      <c r="B36" s="61"/>
       <c r="C36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
       <c r="F36" s="14" t="s">
         <v>50</v>
       </c>
@@ -2525,34 +2540,6 @@
   </sheetData>
   <autoFilter ref="F4:O36"/>
   <mergeCells count="44">
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B12:B22"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F2:N2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B2:E4"/>
     <mergeCell ref="B30:B36"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D14:E14"/>
@@ -2569,6 +2556,34 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F2:N2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B2:E4"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B12:B22"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>

</xml_diff>